<commit_message>
union the power and twi connector in fingerboard eceshop version. finished commercial (china) version of fingerboard
</commit_message>
<xml_diff>
--- a/PCB/Project Outputs for RF Board/RF Board.xlsx
+++ b/PCB/Project Outputs for RF Board/RF Board.xlsx
@@ -497,8 +497,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="26.85546875" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1"/>
+    <col min="1" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changes to mainboard, change to reset circuit, add NMI for usb bootloader
</commit_message>
<xml_diff>
--- a/PCB/Project Outputs for RF Board/RF Board.xlsx
+++ b/PCB/Project Outputs for RF Board/RF Board.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14625"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="10290"/>
   </bookViews>
   <sheets>
     <sheet name="RF Board" sheetId="1" r:id="rId1"/>
@@ -497,8 +497,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="1" max="6" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>